<commit_message>
Updated shrcore IG to objective FHIR 6.0 IG
</commit_message>
<xml_diff>
--- a/docs/shrcore/shr-core-Address-extension.xlsx
+++ b/docs/shrcore/shr-core-Address-extension.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="70">
   <si>
     <t>Path</t>
   </si>
@@ -138,30 +138,30 @@
   </si>
   <si>
     <t>An address expressed using postal conventions (as opposed to GPS or other location definition formats). This data type may be used to convey addresses for use in delivering mail as well as for visiting locations and which might not be valid for mail delivery. There are a variety of postal address formats defined around the world. (Source: HL7 FHIR).</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {children().count() &gt; id.count()}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Extension.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -170,11 +170,31 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>Element.extension</t>
@@ -183,7 +203,7 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -193,20 +213,23 @@
     <t>Source of the definition for the extension code - a logical name or a URL.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Address-extension"/&gt;</t>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/obf/StructureDefinition/shr-core-Address-extension</t>
   </si>
   <si>
     <t>Extension.valueAddress</t>
   </si>
   <si>
-    <t xml:space="preserve">Address {[]} {[]}
+    <t xml:space="preserve">Address
 </t>
   </si>
   <si>
     <t>Value of extension</t>
   </si>
   <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](extensibility.html) for a list).</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -262,67 +285,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -369,7 +392,7 @@
   <cols>
     <col min="1" max="1" width="22.2578125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
@@ -377,7 +400,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.0859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.421875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -394,7 +417,7 @@
     <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
@@ -599,18 +622,18 @@
         <v>37</v>
       </c>
       <c r="AG2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AH2" t="s" s="2">
+      <c r="AI2" t="s" s="2">
         <v>42</v>
-      </c>
-      <c r="AI2" t="s" s="2">
-        <v>43</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -621,7 +644,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>36</v>
@@ -696,7 +719,7 @@
         <v>37</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>36</v>
@@ -711,7 +734,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
@@ -730,15 +753,17 @@
         <v>36</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>54</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>36</v>
@@ -775,19 +800,19 @@
         <v>36</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>37</v>
@@ -804,7 +829,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -812,10 +837,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>36</v>
@@ -827,22 +852,24 @@
         <v>36</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>63</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>36</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>36</v>
@@ -884,13 +911,13 @@
         <v>36</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>36</v>
@@ -901,7 +928,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -909,10 +936,10 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>36</v>
@@ -924,13 +951,13 @@
         <v>36</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -981,13 +1008,13 @@
         <v>36</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>36</v>

</xml_diff>